<commit_message>
While loops crash program, can't think of how to complete the program without one.
</commit_message>
<xml_diff>
--- a/FINAL_PROJECT_Gerrit_Kat_04_16_2022.xlsx
+++ b/FINAL_PROJECT_Gerrit_Kat_04_16_2022.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25028"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="V:\Derek\PROG280-Resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Programming\School Projects\PROG 280 - Advanced Programming\Blackjack-Game\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E6B7507-A1E5-4D64-894E-8774B4E047C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LOG" sheetId="1" r:id="rId1"/>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="48">
   <si>
     <t>Task</t>
   </si>
@@ -115,12 +116,66 @@
   </si>
   <si>
     <t>Struggling on where to begin this task</t>
+  </si>
+  <si>
+    <t>Design Forms</t>
+  </si>
+  <si>
+    <t>Designing the forms to display controls for the user</t>
+  </si>
+  <si>
+    <t>Create AI</t>
+  </si>
+  <si>
+    <t>Offline Functionality</t>
+  </si>
+  <si>
+    <t>Create an AI player to compete with the player offline</t>
+  </si>
+  <si>
+    <t>Basic Functionality</t>
+  </si>
+  <si>
+    <t>Create TCP Connection</t>
+  </si>
+  <si>
+    <t>Establish a connection between players</t>
+  </si>
+  <si>
+    <t>Create User Classes</t>
+  </si>
+  <si>
+    <t>User Accounts</t>
+  </si>
+  <si>
+    <t>2 hours</t>
+  </si>
+  <si>
+    <t>Create Card/Deck Classes</t>
+  </si>
+  <si>
+    <t>Created card class with constructor, created deck with option to add cards and method to shuffle the deck.</t>
+  </si>
+  <si>
+    <t>30 mins</t>
+  </si>
+  <si>
+    <t>Add classes to manage the cards in a deck and shuffle them for randomization.</t>
+  </si>
+  <si>
+    <t>Created the starting form with buttons to begin types of games, added background images to both the starting form and the game board form.</t>
+  </si>
+  <si>
+    <t>Create Dealing Cards Methods</t>
+  </si>
+  <si>
+    <t>Created basic "dealer rules" AI that stands on 17 or higher and hits below that.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -197,6 +252,9 @@
   </cellStyleXfs>
   <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -205,9 +263,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -276,30 +331,30 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A2:F187" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8">
-  <autoFilter ref="A2:F187"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table2" displayName="Table2" ref="A2:F186" totalsRowShown="0" headerRowDxfId="15" dataDxfId="14">
+  <autoFilter ref="A2:F186" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
   <tableColumns count="6">
-    <tableColumn id="1" name="Task" dataDxfId="15"/>
-    <tableColumn id="2" name="Feature" dataDxfId="14"/>
-    <tableColumn id="3" name="Status" dataDxfId="13"/>
-    <tableColumn id="4" name="Duration" dataDxfId="12"/>
-    <tableColumn id="5" name="Description" dataDxfId="11"/>
-    <tableColumn id="6" name="Comments" dataDxfId="10"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Task" dataDxfId="13"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Feature" dataDxfId="12"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Status" dataDxfId="11"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Duration" dataDxfId="10"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Description" dataDxfId="9"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Comments" dataDxfId="8"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table24" displayName="Table24" ref="A2:F187" totalsRowShown="0" headerRowDxfId="1" dataDxfId="0">
-  <autoFilter ref="A2:F187"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table24" displayName="Table24" ref="A2:F187" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
+  <autoFilter ref="A2:F187" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
   <tableColumns count="6">
-    <tableColumn id="1" name="Task" dataDxfId="7"/>
-    <tableColumn id="2" name="Feature" dataDxfId="6"/>
-    <tableColumn id="3" name="Status" dataDxfId="5"/>
-    <tableColumn id="4" name="Duration" dataDxfId="4"/>
-    <tableColumn id="5" name="Description" dataDxfId="3"/>
-    <tableColumn id="6" name="Comments" dataDxfId="2"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Task" dataDxfId="5"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Feature" dataDxfId="4"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="Status" dataDxfId="3"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="Duration" dataDxfId="2"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0100-000005000000}" name="Description" dataDxfId="1"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0100-000006000000}" name="Comments" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -567,51 +622,141 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.5703125" style="4" customWidth="1"/>
-    <col min="2" max="2" width="17.42578125" style="4" customWidth="1"/>
-    <col min="3" max="3" width="17.5703125" style="4" customWidth="1"/>
-    <col min="4" max="4" width="37.42578125" style="4" customWidth="1"/>
-    <col min="5" max="5" width="17.5703125" style="4" customWidth="1"/>
-    <col min="6" max="6" width="20.85546875" style="4" customWidth="1"/>
+    <col min="1" max="1" width="15.5703125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="17.42578125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="17.5703125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="37.42578125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="17.5703125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="20.85546875" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="36.75" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="3"/>
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="4"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="E2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="F2" s="1" t="s">
         <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="105" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="90" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>46</v>
       </c>
     </row>
   </sheetData>
@@ -627,7 +772,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -636,118 +781,118 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.5703125" style="4" customWidth="1"/>
-    <col min="2" max="2" width="17.42578125" style="4" customWidth="1"/>
-    <col min="3" max="3" width="17.5703125" style="4" customWidth="1"/>
-    <col min="4" max="4" width="37.42578125" style="4" customWidth="1"/>
-    <col min="5" max="5" width="17.5703125" style="4" customWidth="1"/>
-    <col min="6" max="6" width="20.85546875" style="4" customWidth="1"/>
+    <col min="1" max="1" width="15.5703125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="17.42578125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="17.5703125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="37.42578125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="17.5703125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="20.85546875" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="36.75" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="3"/>
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="4"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="E2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="F2" s="1" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="D3" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="E3" s="4" t="s">
+      <c r="E3" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F3" s="4" t="s">
+      <c r="F3" s="1" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
+      <c r="A4" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B4" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C4" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="D4" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E4" s="4" t="s">
+      <c r="E4" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="F4" s="4" t="s">
+      <c r="F4" s="1" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="90" x14ac:dyDescent="0.25">
-      <c r="A5" s="4" t="s">
+      <c r="A5" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B5" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="C5" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D5" s="4" t="s">
+      <c r="D5" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="E5" s="4" t="s">
+      <c r="E5" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="F5" s="4" t="s">
+      <c r="F5" s="1" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A6" s="4" t="s">
+      <c r="A6" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="B6" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="C6" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="E6" s="4" t="s">
+      <c r="E6" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="F6" s="4" t="s">
+      <c r="F6" s="1" t="s">
         <v>29</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Attempted some resolution of the while loop freeze, no luck so far.
</commit_message>
<xml_diff>
--- a/FINAL_PROJECT_Gerrit_Kat_04_16_2022.xlsx
+++ b/FINAL_PROJECT_Gerrit_Kat_04_16_2022.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Programming\School Projects\PROG 280 - Advanced Programming\Blackjack-Game\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E6B7507-A1E5-4D64-894E-8774B4E047C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B6CA0EF-3C7E-4C38-80AF-ADA572565546}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="49">
   <si>
     <t>Task</t>
   </si>
@@ -170,6 +170,9 @@
   </si>
   <si>
     <t>Created basic "dealer rules" AI that stands on 17 or higher and hits below that.</t>
+  </si>
+  <si>
+    <t>1 hour</t>
   </si>
 </sst>
 </file>
@@ -626,7 +629,7 @@
   <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -757,6 +760,15 @@
     <row r="8" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>46</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>48</v>
       </c>
     </row>
   </sheetData>

</xml_diff>